<commit_message>
feat: Find instances with all disagreeing annotators
</commit_message>
<xml_diff>
--- a/DataSetExplorer/DataSetSerializer/Template/Dataset Annotation Template.xlsx
+++ b/DataSetExplorer/DataSetSerializer/Template/Dataset Annotation Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubur\Documents\Fakultet\!PROJEKTI\Clean CaDET\PLATFORM\platform-repository-compiler\DataSetExplorer\DataSetSerializer\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B066E3BA-CBC1-42C5-93E7-3352EEFF1BAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619D1A64-B018-439C-BF97-D84803E4FD71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -474,9 +474,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
@@ -516,7 +514,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0,1,2,3"</formula1>
     </dataValidation>

</xml_diff>